<commit_message>
Ajout dimensions du logo Pokémon
</commit_message>
<xml_diff>
--- a/Charte Graphique.xlsx
+++ b/Charte Graphique.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjetIHM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="576" yWindow="84" windowWidth="15876" windowHeight="5856"/>
+    <workbookView xWindow="570" yWindow="90" windowWidth="15870" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>Fond</t>
   </si>
@@ -115,13 +120,16 @@
   </si>
   <si>
     <t>Taille</t>
+  </si>
+  <si>
+    <t>1023x640</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,11 +144,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -308,6 +311,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -351,15 +357,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>281940</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
+          <xdr:colOff>466725</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -372,7 +378,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -380,6 +386,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -392,15 +421,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>274320</xdr:colOff>
+          <xdr:colOff>276225</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -413,7 +442,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -421,6 +450,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -433,15 +485,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>289560</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>472440</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -454,7 +506,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -462,6 +514,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -476,11 +551,11 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>449580</xdr:colOff>
+          <xdr:colOff>447675</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -495,7 +570,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -503,6 +578,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -515,13 +613,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>289560</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>472440</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -536,7 +634,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -544,6 +642,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -556,13 +677,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>327660</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -577,7 +698,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -585,6 +706,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -597,15 +741,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>312420</xdr:colOff>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>55</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>56</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -618,7 +762,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -626,6 +770,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -638,13 +805,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>327660</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -659,7 +826,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -667,6 +834,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -720,7 +910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,7 +945,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -966,31 +1156,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -999,7 +1189,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1008,20 +1198,22 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1030,7 +1222,7 @@
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1039,13 +1231,13 @@
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1246,7 @@
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1063,42 +1255,42 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1299,7 @@
       </c>
       <c r="C17" s="14"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1116,42 +1308,42 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1352,7 @@
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1169,42 +1361,42 @@
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1405,7 @@
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1222,42 +1414,42 @@
       </c>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1458,7 @@
       </c>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1275,42 +1467,42 @@
       </c>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1322,7 +1514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1334,35 +1526,35 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -1371,14 +1563,14 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1579,7 @@
       </c>
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1396,28 +1588,28 @@
       </c>
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>27</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -1442,15 +1634,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>281940</xdr:colOff>
+                    <xdr:colOff>285750</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
+                    <xdr:colOff>466725</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1464,15 +1656,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>274320</xdr:colOff>
+                    <xdr:colOff>276225</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1486,15 +1678,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>289560</xdr:colOff>
+                    <xdr:colOff>285750</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>472440</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1510,11 +1702,11 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:colOff>447675</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1530,13 +1722,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>289560</xdr:colOff>
+                    <xdr:colOff>285750</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>472440</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>34</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1552,13 +1744,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>327660</xdr:colOff>
+                    <xdr:colOff>323850</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>510540</xdr:colOff>
+                    <xdr:colOff>514350</xdr:colOff>
                     <xdr:row>41</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1574,15 +1766,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>312420</xdr:colOff>
+                    <xdr:colOff>314325</xdr:colOff>
                     <xdr:row>55</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>56</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1596,13 +1788,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>327660</xdr:colOff>
+                    <xdr:colOff>323850</xdr:colOff>
                     <xdr:row>47</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>510540</xdr:colOff>
+                    <xdr:colOff>514350</xdr:colOff>
                     <xdr:row>48</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1623,7 +1815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1635,7 +1827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#Pokemon# [Projet] Style Edit Combat interface
</commit_message>
<xml_diff>
--- a/Charte Graphique.xlsx
+++ b/Charte Graphique.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="84" windowWidth="15876" windowHeight="5856"/>
+    <workbookView xWindow="570" yWindow="90" windowWidth="15870" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>Fond</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>Taille</t>
+  </si>
+  <si>
+    <t>#993300</t>
+  </si>
+  <si>
+    <t>#662200</t>
+  </si>
+  <si>
+    <t>#0000FF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,11 +145,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -351,15 +355,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>281940</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
+          <xdr:colOff>466725</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -392,15 +396,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>274320</xdr:colOff>
+          <xdr:colOff>276225</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -433,15 +437,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>289560</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>472440</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -476,11 +480,11 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>449580</xdr:colOff>
+          <xdr:colOff>447675</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -515,13 +519,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>289560</xdr:colOff>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>472440</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -556,13 +560,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>327660</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -597,15 +601,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>312420</xdr:colOff>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>55</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>56</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -638,13 +642,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>327660</xdr:colOff>
+          <xdr:colOff>323850</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -966,31 +970,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -999,7 +1003,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1008,20 +1012,20 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1030,7 +1034,7 @@
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1039,13 +1043,13 @@
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1058,7 @@
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1063,42 +1067,42 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1111,7 @@
       </c>
       <c r="C17" s="14"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1116,42 +1120,42 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1164,7 @@
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1169,42 +1173,42 @@
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1217,7 @@
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1222,147 +1226,147 @@
       </c>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -1371,23 +1375,23 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1396,28 +1400,28 @@
       </c>
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>27</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>25</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -1442,15 +1446,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>281940</xdr:colOff>
+                    <xdr:colOff>285750</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
+                    <xdr:colOff>466725</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1464,15 +1468,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>274320</xdr:colOff>
+                    <xdr:colOff>276225</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1486,15 +1490,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>289560</xdr:colOff>
+                    <xdr:colOff>285750</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>472440</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1510,11 +1514,11 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>449580</xdr:colOff>
+                    <xdr:colOff>447675</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1530,13 +1534,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>289560</xdr:colOff>
+                    <xdr:colOff>285750</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>472440</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>34</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1552,13 +1556,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>327660</xdr:colOff>
+                    <xdr:colOff>323850</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>510540</xdr:colOff>
+                    <xdr:colOff>514350</xdr:colOff>
                     <xdr:row>41</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1574,15 +1578,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>312420</xdr:colOff>
+                    <xdr:colOff>314325</xdr:colOff>
                     <xdr:row>55</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>56</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1596,13 +1600,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>327660</xdr:colOff>
+                    <xdr:colOff>323850</xdr:colOff>
                     <xdr:row>47</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>510540</xdr:colOff>
+                    <xdr:colOff>514350</xdr:colOff>
                     <xdr:row>48</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1623,7 +1627,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1635,7 +1639,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Ajout dernières images."
This reverts commit 4eb96814b64a583c5636f9c0a317b188a61a2aa0.
</commit_message>
<xml_diff>
--- a/Charte Graphique.xlsx
+++ b/Charte Graphique.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjetIHM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="570" yWindow="90" windowWidth="15870" windowHeight="5850"/>
+    <workbookView xWindow="576" yWindow="84" windowWidth="15876" windowHeight="5856"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Fond</t>
   </si>
@@ -120,16 +115,13 @@
   </si>
   <si>
     <t>Taille</t>
-  </si>
-  <si>
-    <t>1023x640</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +136,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -311,9 +308,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -357,15 +351,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>285750</xdr:colOff>
+          <xdr:colOff>281940</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>466725</xdr:colOff>
+          <xdr:colOff>464820</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -378,7 +372,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -386,29 +380,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -421,15 +392,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>274320</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -442,7 +413,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -450,29 +421,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -485,15 +433,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>285750</xdr:colOff>
+          <xdr:colOff>289560</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>472440</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -506,7 +454,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -514,29 +462,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -551,11 +476,11 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>447675</xdr:colOff>
+          <xdr:colOff>449580</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -570,7 +495,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -578,29 +503,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -613,13 +515,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>285750</xdr:colOff>
+          <xdr:colOff>289560</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>472440</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -634,7 +536,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -642,29 +544,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -677,13 +556,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>323850</xdr:colOff>
+          <xdr:colOff>327660</xdr:colOff>
           <xdr:row>40</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>514350</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -698,7 +577,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -706,29 +585,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -741,15 +597,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>314325</xdr:colOff>
+          <xdr:colOff>312420</xdr:colOff>
           <xdr:row>55</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>56</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -762,7 +618,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -770,29 +626,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -805,13 +638,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>323850</xdr:colOff>
+          <xdr:colOff>327660</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>514350</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -826,7 +659,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -834,29 +667,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -910,7 +720,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -945,7 +755,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1156,31 +966,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +999,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1198,22 +1008,20 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1222,7 +1030,7 @@
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1231,13 +1039,13 @@
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1054,7 @@
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1255,42 +1063,42 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1107,7 @@
       </c>
       <c r="C17" s="14"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1308,42 +1116,42 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1160,7 @@
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1361,42 +1169,42 @@
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1213,7 @@
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1414,42 +1222,42 @@
       </c>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1266,7 @@
       </c>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1467,42 +1275,42 @@
       </c>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>27</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1514,7 +1322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1526,35 +1334,35 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -1563,14 +1371,14 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1387,7 @@
       </c>
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1588,28 +1396,28 @@
       </c>
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>27</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>25</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -1634,15 +1442,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>285750</xdr:colOff>
+                    <xdr:colOff>281940</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>466725</xdr:colOff>
+                    <xdr:colOff>464820</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1656,15 +1464,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:colOff>274320</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1678,15 +1486,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>285750</xdr:colOff>
+                    <xdr:colOff>289560</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>472440</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1702,11 +1510,11 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>447675</xdr:colOff>
+                    <xdr:colOff>449580</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1722,13 +1530,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>285750</xdr:colOff>
+                    <xdr:colOff>289560</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>472440</xdr:colOff>
                     <xdr:row>34</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1744,13 +1552,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>323850</xdr:colOff>
+                    <xdr:colOff>327660</xdr:colOff>
                     <xdr:row>40</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:colOff>510540</xdr:colOff>
                     <xdr:row>41</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1766,15 +1574,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:colOff>312420</xdr:colOff>
                     <xdr:row>55</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>56</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1788,13 +1596,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>323850</xdr:colOff>
+                    <xdr:colOff>327660</xdr:colOff>
                     <xdr:row>47</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:colOff>510540</xdr:colOff>
                     <xdr:row>48</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1815,7 +1623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1827,7 +1635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#Pokemon# [Mathieu] Create Button Back Need Maxime Styles update Create Button Folder
</commit_message>
<xml_diff>
--- a/Charte Graphique.xlsx
+++ b/Charte Graphique.xlsx
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1300,7 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -1314,7 +1314,7 @@
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1338,28 +1338,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -1375,14 +1375,14 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1400,28 +1400,28 @@
       </c>
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>27</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Ajout de la carte entière. Possibilité de bouger le personnage sur la carte. Ajout des styles nécessaires. Mise en place du menu sur la droite de l'écran et ajout des boutons qui permettront de consulter les différents pokémons, sac, etc...
</commit_message>
<xml_diff>
--- a/Charte Graphique.xlsx
+++ b/Charte Graphique.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjetIHM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="570" yWindow="90" windowWidth="15870" windowHeight="5850"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>Fond</t>
   </si>
@@ -124,6 +129,27 @@
   </si>
   <si>
     <t>#0000FF</t>
+  </si>
+  <si>
+    <t>#4388CC</t>
+  </si>
+  <si>
+    <t>Bouton menu pokédex</t>
+  </si>
+  <si>
+    <t>Bouton menu pokémon</t>
+  </si>
+  <si>
+    <t>Bouton menu personnage</t>
+  </si>
+  <si>
+    <t>#993399</t>
+  </si>
+  <si>
+    <t>Bouton menu sac</t>
+  </si>
+  <si>
+    <t>#FF9900</t>
   </si>
 </sst>
 </file>
@@ -266,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,6 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,11 +339,26 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -348,6 +390,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -376,7 +422,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -384,6 +430,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -417,7 +486,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -425,6 +494,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -458,7 +550,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -466,6 +558,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -499,7 +614,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -507,6 +622,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -540,7 +678,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -548,6 +686,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -581,7 +742,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -589,6 +750,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -622,7 +806,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -630,6 +814,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -663,7 +870,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -671,6 +878,285 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>314325</xdr:colOff>
+          <xdr:row>63</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>495300</xdr:colOff>
+          <xdr:row>64</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>314325</xdr:colOff>
+          <xdr:row>71</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>495300</xdr:colOff>
+          <xdr:row>72</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>314325</xdr:colOff>
+          <xdr:row>79</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>495300</xdr:colOff>
+          <xdr:row>80</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>314325</xdr:colOff>
+          <xdr:row>87</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>495300</xdr:colOff>
+          <xdr:row>88</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -724,7 +1210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -759,7 +1245,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -968,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,8 +1470,8 @@
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1427,6 +1913,189 @@
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="18"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="18"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>25</v>
+      </c>
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="3"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>27</v>
+      </c>
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1615,6 +2284,94 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId12" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>63</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>495300</xdr:colOff>
+                    <xdr:row>64</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId13" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>71</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>495300</xdr:colOff>
+                    <xdr:row>72</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId14" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>79</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>495300</xdr:colOff>
+                    <xdr:row>80</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId15" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:row>87</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>495300</xdr:colOff>
+                    <xdr:row>88</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>